<commit_message>
started on excel parsing
</commit_message>
<xml_diff>
--- a/excel01.xlsx
+++ b/excel01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\GitHub\Markdownify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62C766CA-74F0-405B-B15C-3C9EFA61562D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA04A49-CF29-4BB7-9211-48AE170CDED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23385" yWindow="2595" windowWidth="29040" windowHeight="16410" xr2:uid="{59577EC4-1014-42DD-8D42-0CDEA795D458}"/>
+    <workbookView xWindow="-23385" yWindow="2340" windowWidth="29040" windowHeight="16410" xr2:uid="{59577EC4-1014-42DD-8D42-0CDEA795D458}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,25 +34,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+  <si>
+    <t>HolyFuck</t>
+  </si>
+  <si>
+    <t>ShitBalls</t>
+  </si>
+  <si>
+    <t>C1R1</t>
+  </si>
+  <si>
+    <t>C1R2</t>
+  </si>
+  <si>
+    <t>C1R3</t>
+  </si>
+  <si>
+    <t>C2R1</t>
+  </si>
+  <si>
+    <t>C2R2</t>
+  </si>
+  <si>
+    <t>C3R3</t>
+  </si>
+  <si>
+    <t>C3R1</t>
+  </si>
+  <si>
+    <t>C3R2</t>
+  </si>
+  <si>
+    <t>C1R4</t>
+  </si>
+  <si>
+    <t>C2R3</t>
+  </si>
+  <si>
+    <t>C3R4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -394,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7824393E-6B9E-42F2-A62B-0EE98EAEAD5E}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,43 +446,55 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>3</v>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-      <c r="C3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>9</v>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
started on reading content
</commit_message>
<xml_diff>
--- a/excel01.xlsx
+++ b/excel01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\GitHub\Markdownify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA04A49-CF29-4BB7-9211-48AE170CDED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A0651A-4CE0-4554-8694-BCFFF20498D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23385" yWindow="2340" windowWidth="29040" windowHeight="16410" xr2:uid="{59577EC4-1014-42DD-8D42-0CDEA795D458}"/>
   </bookViews>
@@ -433,7 +433,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added basic table converter for Excel
</commit_message>
<xml_diff>
--- a/excel01.xlsx
+++ b/excel01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\GitHub\Markdownify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A0651A-4CE0-4554-8694-BCFFF20498D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14874A3-B671-48C9-A8EA-71AC3DF1CB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23385" yWindow="2340" windowWidth="29040" windowHeight="16410" xr2:uid="{59577EC4-1014-42DD-8D42-0CDEA795D458}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{59577EC4-1014-42DD-8D42-0CDEA795D458}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
-    <t>HolyFuck</t>
-  </si>
-  <si>
-    <t>ShitBalls</t>
-  </si>
-  <si>
     <t>C1R1</t>
   </si>
   <si>
@@ -73,6 +67,12 @@
   </si>
   <si>
     <t>C3R4</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>Heading</t>
   </si>
 </sst>
 </file>
@@ -433,64 +433,64 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>